<commit_message>
Actualizando Archivo de Excel para visualizacion
</commit_message>
<xml_diff>
--- a/ProyectosEjemplo.xlsx
+++ b/ProyectosEjemplo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulloa\Desktop\Proyectos Desarrollo\ChatBotXOne\AppChatBotXOne - Dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panch\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB48D99A-473A-4181-A17D-4269CFD6EDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D02581E-458B-4C0C-9636-9BD2553D3C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15AA1E02-0B31-4ADF-81E4-BED79850A1EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="286">
   <si>
     <t>TABLA DE DESCUENTOS SEGÚN VOLUMEN DE COMPRA</t>
   </si>
@@ -285,9 +285,6 @@
   </si>
   <si>
     <t>AUTOMATIZACION DE MINIMO BODEGA CENTRAL</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>MARIA JOSE POZO</t>
@@ -917,12 +914,15 @@
   <si>
     <t>FECHA ESTIMADA DEL PRIMER PILOTO</t>
   </si>
+  <si>
+    <t>PENDIENTE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -943,6 +943,14 @@
       <color theme="0"/>
       <name val="Biome"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -997,7 +1005,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1014,6 +1022,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1372,10 +1381,10 @@
   <dimension ref="A1:T55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="129.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="255.6640625" bestFit="1" customWidth="1"/>
@@ -1385,66 +1394,69 @@
     <col min="20" max="20" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="34.5" customHeight="1">
+    <row r="1" spans="1:20" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>285</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="T1" s="5" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1491,22 +1503,22 @@
         <v>6</v>
       </c>
       <c r="P2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q2" t="s">
         <v>7</v>
       </c>
       <c r="R2" t="s">
+        <v>198</v>
+      </c>
+      <c r="S2" t="s">
         <v>199</v>
-      </c>
-      <c r="S2" t="s">
-        <v>200</v>
       </c>
       <c r="T2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4</v>
       </c>
@@ -1553,22 +1565,22 @@
         <v>6</v>
       </c>
       <c r="P3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q3" t="s">
         <v>13</v>
       </c>
       <c r="R3" t="s">
+        <v>200</v>
+      </c>
+      <c r="S3" t="s">
         <v>201</v>
-      </c>
-      <c r="S3" t="s">
-        <v>202</v>
       </c>
       <c r="T3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5</v>
       </c>
@@ -1615,27 +1627,27 @@
         <v>6</v>
       </c>
       <c r="P4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q4" t="s">
         <v>13</v>
       </c>
       <c r="R4" t="s">
+        <v>202</v>
+      </c>
+      <c r="S4" t="s">
         <v>203</v>
-      </c>
-      <c r="S4" t="s">
-        <v>204</v>
       </c>
       <c r="T4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -1677,19 +1689,22 @@
         <v>21</v>
       </c>
       <c r="P5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q5" t="s">
         <v>22</v>
       </c>
       <c r="R5" t="s">
+        <v>206</v>
+      </c>
+      <c r="S5" t="s">
         <v>207</v>
       </c>
-      <c r="S5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="T5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>8</v>
       </c>
@@ -1736,22 +1751,22 @@
         <v>21</v>
       </c>
       <c r="P6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q6" t="s">
         <v>25</v>
       </c>
       <c r="R6" t="s">
+        <v>208</v>
+      </c>
+      <c r="S6" t="s">
         <v>209</v>
-      </c>
-      <c r="S6" t="s">
-        <v>210</v>
       </c>
       <c r="T6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1798,22 +1813,22 @@
         <v>31</v>
       </c>
       <c r="P7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q7" t="s">
         <v>32</v>
       </c>
       <c r="R7" t="s">
+        <v>210</v>
+      </c>
+      <c r="S7" t="s">
         <v>211</v>
-      </c>
-      <c r="S7" t="s">
-        <v>212</v>
       </c>
       <c r="T7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10</v>
       </c>
@@ -1860,22 +1875,22 @@
         <v>31</v>
       </c>
       <c r="P8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q8" t="s">
         <v>38</v>
       </c>
       <c r="R8" t="s">
+        <v>212</v>
+      </c>
+      <c r="S8" t="s">
         <v>213</v>
-      </c>
-      <c r="S8" t="s">
-        <v>214</v>
       </c>
       <c r="T8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>12</v>
       </c>
@@ -1922,13 +1937,22 @@
         <v>6</v>
       </c>
       <c r="P9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="R9" t="s">
+        <v>285</v>
+      </c>
+      <c r="S9" t="s">
+        <v>285</v>
+      </c>
+      <c r="T9" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>13</v>
       </c>
@@ -1975,19 +1999,22 @@
         <v>31</v>
       </c>
       <c r="P10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q10" t="s">
         <v>32</v>
       </c>
       <c r="R10" t="s">
+        <v>214</v>
+      </c>
+      <c r="S10" t="s">
         <v>215</v>
       </c>
-      <c r="S10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="T10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>14</v>
       </c>
@@ -2034,19 +2061,22 @@
         <v>31</v>
       </c>
       <c r="P11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q11" t="s">
         <v>32</v>
       </c>
       <c r="R11" t="s">
+        <v>216</v>
+      </c>
+      <c r="S11" t="s">
         <v>217</v>
       </c>
-      <c r="S11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="T11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>16</v>
       </c>
@@ -2093,13 +2123,22 @@
         <v>52</v>
       </c>
       <c r="P12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="R12" t="s">
+        <v>285</v>
+      </c>
+      <c r="S12" t="s">
+        <v>285</v>
+      </c>
+      <c r="T12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>18</v>
       </c>
@@ -2146,19 +2185,22 @@
         <v>52</v>
       </c>
       <c r="P13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q13" t="s">
         <v>56</v>
       </c>
       <c r="R13" t="s">
+        <v>218</v>
+      </c>
+      <c r="S13" t="s">
         <v>219</v>
       </c>
-      <c r="S13" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="T13" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>19</v>
       </c>
@@ -2205,13 +2247,22 @@
         <v>52</v>
       </c>
       <c r="P14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="R14" t="s">
+        <v>285</v>
+      </c>
+      <c r="S14" t="s">
+        <v>285</v>
+      </c>
+      <c r="T14" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>20</v>
       </c>
@@ -2258,13 +2309,22 @@
         <v>52</v>
       </c>
       <c r="P15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q15" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="R15" t="s">
+        <v>285</v>
+      </c>
+      <c r="S15" t="s">
+        <v>285</v>
+      </c>
+      <c r="T15" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>21</v>
       </c>
@@ -2311,13 +2371,22 @@
         <v>52</v>
       </c>
       <c r="P16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="R16" t="s">
+        <v>285</v>
+      </c>
+      <c r="S16" t="s">
+        <v>285</v>
+      </c>
+      <c r="T16" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>22</v>
       </c>
@@ -2364,22 +2433,22 @@
         <v>66</v>
       </c>
       <c r="P17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q17" t="s">
         <v>67</v>
       </c>
       <c r="R17" t="s">
+        <v>220</v>
+      </c>
+      <c r="S17" t="s">
         <v>221</v>
-      </c>
-      <c r="S17" t="s">
-        <v>222</v>
       </c>
       <c r="T17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>23</v>
       </c>
@@ -2426,22 +2495,22 @@
         <v>6</v>
       </c>
       <c r="P18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q18" t="s">
         <v>7</v>
       </c>
       <c r="R18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="S18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>24</v>
       </c>
@@ -2488,19 +2557,22 @@
         <v>6</v>
       </c>
       <c r="P19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q19" t="s">
         <v>7</v>
       </c>
       <c r="R19" t="s">
-        <v>224</v>
+        <v>223</v>
+      </c>
+      <c r="S19" t="s">
+        <v>285</v>
       </c>
       <c r="T19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>25</v>
       </c>
@@ -2547,7 +2619,7 @@
         <v>52</v>
       </c>
       <c r="P20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q20" t="s">
         <v>79</v>
@@ -2555,19 +2627,25 @@
       <c r="R20" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="1:20">
+      <c r="S20" t="s">
+        <v>285</v>
+      </c>
+      <c r="T20" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>26</v>
       </c>
       <c r="B21" t="s">
         <v>81</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D21" t="s">
         <v>82</v>
-      </c>
-      <c r="D21" t="s">
-        <v>83</v>
       </c>
       <c r="E21" t="s">
         <v>55</v>
@@ -2599,22 +2677,34 @@
       <c r="N21">
         <v>0.35</v>
       </c>
+      <c r="O21" t="s">
+        <v>285</v>
+      </c>
       <c r="P21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q21" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:20">
+      <c r="R21" t="s">
+        <v>285</v>
+      </c>
+      <c r="S21" t="s">
+        <v>285</v>
+      </c>
+      <c r="T21" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>27</v>
       </c>
       <c r="B22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" t="s">
         <v>84</v>
-      </c>
-      <c r="C22" t="s">
-        <v>85</v>
       </c>
       <c r="D22" t="s">
         <v>54</v>
@@ -2653,39 +2743,39 @@
         <v>52</v>
       </c>
       <c r="P22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q22" t="s">
         <v>56</v>
       </c>
       <c r="R22" t="s">
+        <v>224</v>
+      </c>
+      <c r="S22" t="s">
         <v>225</v>
       </c>
-      <c r="S22" t="s">
-        <v>226</v>
-      </c>
       <c r="T22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>28</v>
       </c>
       <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" t="s">
         <v>87</v>
-      </c>
-      <c r="C23" t="s">
-        <v>88</v>
       </c>
       <c r="D23" t="s">
         <v>78</v>
       </c>
       <c r="E23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" t="s">
         <v>89</v>
-      </c>
-      <c r="F23" t="s">
-        <v>90</v>
       </c>
       <c r="G23">
         <v>8</v>
@@ -2715,18 +2805,30 @@
         <v>52</v>
       </c>
       <c r="P23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q23" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="24" spans="1:20">
+      <c r="R23" t="s">
+        <v>285</v>
+      </c>
+      <c r="S23" t="s">
+        <v>285</v>
+      </c>
+      <c r="T23" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="C24" t="s">
+        <v>285</v>
       </c>
       <c r="D24" t="s">
         <v>51</v>
@@ -2737,6 +2839,21 @@
       <c r="F24" t="s">
         <v>30</v>
       </c>
+      <c r="G24" t="s">
+        <v>285</v>
+      </c>
+      <c r="H24" t="s">
+        <v>285</v>
+      </c>
+      <c r="I24" t="s">
+        <v>285</v>
+      </c>
+      <c r="J24" t="s">
+        <v>285</v>
+      </c>
+      <c r="K24" t="s">
+        <v>285</v>
+      </c>
       <c r="L24">
         <v>0</v>
       </c>
@@ -2746,31 +2863,37 @@
       <c r="N24">
         <v>0.90000000000000013</v>
       </c>
+      <c r="O24" t="s">
+        <v>285</v>
+      </c>
       <c r="P24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q24" t="s">
         <v>56</v>
       </c>
       <c r="R24" t="s">
+        <v>226</v>
+      </c>
+      <c r="S24" t="s">
         <v>227</v>
-      </c>
-      <c r="S24" t="s">
-        <v>228</v>
       </c>
       <c r="T24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>30</v>
       </c>
       <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
+        <v>285</v>
+      </c>
+      <c r="D25" t="s">
         <v>93</v>
-      </c>
-      <c r="D25" t="s">
-        <v>94</v>
       </c>
       <c r="E25" t="s">
         <v>55</v>
@@ -2778,6 +2901,21 @@
       <c r="F25" t="s">
         <v>30</v>
       </c>
+      <c r="G25" t="s">
+        <v>285</v>
+      </c>
+      <c r="H25" t="s">
+        <v>285</v>
+      </c>
+      <c r="I25" t="s">
+        <v>285</v>
+      </c>
+      <c r="J25" t="s">
+        <v>285</v>
+      </c>
+      <c r="K25" t="s">
+        <v>285</v>
+      </c>
       <c r="L25">
         <v>0</v>
       </c>
@@ -2787,28 +2925,34 @@
       <c r="N25">
         <v>0.84999999999999987</v>
       </c>
+      <c r="O25" t="s">
+        <v>285</v>
+      </c>
       <c r="P25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q25" t="s">
         <v>56</v>
       </c>
       <c r="R25" t="s">
+        <v>228</v>
+      </c>
+      <c r="S25" t="s">
         <v>229</v>
-      </c>
-      <c r="S25" t="s">
-        <v>230</v>
       </c>
       <c r="T25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="C26" t="s">
+        <v>285</v>
       </c>
       <c r="D26" t="s">
         <v>51</v>
@@ -2819,6 +2963,21 @@
       <c r="F26" t="s">
         <v>30</v>
       </c>
+      <c r="G26" t="s">
+        <v>285</v>
+      </c>
+      <c r="H26" t="s">
+        <v>285</v>
+      </c>
+      <c r="I26" t="s">
+        <v>285</v>
+      </c>
+      <c r="J26" t="s">
+        <v>285</v>
+      </c>
+      <c r="K26" t="s">
+        <v>285</v>
+      </c>
       <c r="L26">
         <v>0</v>
       </c>
@@ -2828,25 +2987,37 @@
       <c r="N26">
         <v>1</v>
       </c>
+      <c r="O26" t="s">
+        <v>285</v>
+      </c>
       <c r="P26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q26" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="27" spans="1:20">
+      <c r="R26" t="s">
+        <v>285</v>
+      </c>
+      <c r="S26" t="s">
+        <v>285</v>
+      </c>
+      <c r="T26" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>33</v>
       </c>
       <c r="B27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" t="s">
         <v>96</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>97</v>
-      </c>
-      <c r="D27" t="s">
-        <v>98</v>
       </c>
       <c r="E27" t="s">
         <v>20</v>
@@ -2882,33 +3053,33 @@
         <v>21</v>
       </c>
       <c r="P27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q27" t="s">
+        <v>98</v>
+      </c>
+      <c r="R27" t="s">
+        <v>230</v>
+      </c>
+      <c r="S27" t="s">
+        <v>231</v>
+      </c>
+      <c r="T27" t="s">
         <v>99</v>
       </c>
-      <c r="R27" t="s">
-        <v>231</v>
-      </c>
-      <c r="S27" t="s">
-        <v>232</v>
-      </c>
-      <c r="T27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20">
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>34</v>
       </c>
       <c r="B28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" t="s">
         <v>101</v>
       </c>
-      <c r="C28" t="s">
-        <v>102</v>
-      </c>
       <c r="D28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E28" t="s">
         <v>20</v>
@@ -2916,6 +3087,21 @@
       <c r="F28" t="s">
         <v>37</v>
       </c>
+      <c r="G28" t="s">
+        <v>285</v>
+      </c>
+      <c r="H28" t="s">
+        <v>285</v>
+      </c>
+      <c r="I28" t="s">
+        <v>285</v>
+      </c>
+      <c r="J28" t="s">
+        <v>285</v>
+      </c>
+      <c r="K28" t="s">
+        <v>285</v>
+      </c>
       <c r="L28">
         <v>0</v>
       </c>
@@ -2925,34 +3111,37 @@
       <c r="N28">
         <v>0.55000000000000004</v>
       </c>
+      <c r="O28" t="s">
+        <v>285</v>
+      </c>
       <c r="P28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q28" t="s">
         <v>13</v>
       </c>
       <c r="R28" t="s">
+        <v>232</v>
+      </c>
+      <c r="S28" t="s">
         <v>233</v>
       </c>
-      <c r="S28" t="s">
-        <v>234</v>
-      </c>
       <c r="T28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>35</v>
       </c>
       <c r="B29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" t="s">
         <v>104</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>105</v>
-      </c>
-      <c r="D29" t="s">
-        <v>106</v>
       </c>
       <c r="E29" t="s">
         <v>3</v>
@@ -2960,6 +3149,21 @@
       <c r="F29" t="s">
         <v>4</v>
       </c>
+      <c r="G29" t="s">
+        <v>285</v>
+      </c>
+      <c r="H29" t="s">
+        <v>285</v>
+      </c>
+      <c r="I29" t="s">
+        <v>285</v>
+      </c>
+      <c r="J29" t="s">
+        <v>285</v>
+      </c>
+      <c r="K29" t="s">
+        <v>285</v>
+      </c>
       <c r="L29">
         <v>0</v>
       </c>
@@ -2969,34 +3173,40 @@
       <c r="N29">
         <v>0.5</v>
       </c>
+      <c r="O29" t="s">
+        <v>285</v>
+      </c>
       <c r="P29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q29" t="s">
         <v>32</v>
       </c>
       <c r="R29" t="s">
+        <v>234</v>
+      </c>
+      <c r="S29" t="s">
         <v>235</v>
       </c>
-      <c r="S29" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20">
+      <c r="T29" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>36</v>
       </c>
       <c r="B30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" t="s">
         <v>107</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>108</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>109</v>
-      </c>
-      <c r="E30" t="s">
-        <v>110</v>
       </c>
       <c r="F30" t="s">
         <v>4</v>
@@ -3020,30 +3230,42 @@
         <v>30</v>
       </c>
       <c r="M30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N30">
         <v>1</v>
       </c>
+      <c r="O30" t="s">
+        <v>285</v>
+      </c>
       <c r="P30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q30" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" spans="1:20">
+      <c r="R30" t="s">
+        <v>285</v>
+      </c>
+      <c r="S30" t="s">
+        <v>285</v>
+      </c>
+      <c r="T30" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>37</v>
       </c>
       <c r="B31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" t="s">
         <v>113</v>
       </c>
-      <c r="C31" t="s">
-        <v>114</v>
-      </c>
       <c r="D31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E31" t="s">
         <v>3</v>
@@ -3070,39 +3292,42 @@
         <v>30</v>
       </c>
       <c r="M31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N31">
         <v>0.2</v>
       </c>
+      <c r="O31" t="s">
+        <v>285</v>
+      </c>
       <c r="P31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q31" t="s">
+        <v>114</v>
+      </c>
+      <c r="R31" t="s">
+        <v>236</v>
+      </c>
+      <c r="S31" t="s">
+        <v>237</v>
+      </c>
+      <c r="T31" t="s">
         <v>115</v>
       </c>
-      <c r="R31" t="s">
-        <v>237</v>
-      </c>
-      <c r="S31" t="s">
-        <v>238</v>
-      </c>
-      <c r="T31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20">
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>38</v>
       </c>
       <c r="B32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" t="s">
         <v>117</v>
       </c>
-      <c r="C32" t="s">
-        <v>118</v>
-      </c>
       <c r="D32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E32" t="s">
         <v>3</v>
@@ -3129,39 +3354,42 @@
         <v>30</v>
       </c>
       <c r="M32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N32">
         <v>0.2</v>
       </c>
+      <c r="O32" t="s">
+        <v>285</v>
+      </c>
       <c r="P32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R32" t="s">
+        <v>238</v>
+      </c>
+      <c r="S32" t="s">
         <v>239</v>
       </c>
-      <c r="S32" t="s">
-        <v>240</v>
-      </c>
       <c r="T32" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>50</v>
       </c>
       <c r="B33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" t="s">
         <v>120</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>121</v>
-      </c>
-      <c r="D33" t="s">
-        <v>122</v>
       </c>
       <c r="E33" t="s">
         <v>3</v>
@@ -3188,39 +3416,42 @@
         <v>20</v>
       </c>
       <c r="M33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N33">
         <v>1.0000000000000002</v>
       </c>
+      <c r="O33" t="s">
+        <v>285</v>
+      </c>
       <c r="P33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q33" t="s">
+        <v>122</v>
+      </c>
+      <c r="R33" t="s">
+        <v>240</v>
+      </c>
+      <c r="S33" t="s">
+        <v>240</v>
+      </c>
+      <c r="T33" t="s">
         <v>123</v>
       </c>
-      <c r="R33" t="s">
-        <v>241</v>
-      </c>
-      <c r="S33" t="s">
-        <v>241</v>
-      </c>
-      <c r="T33" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20">
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>51</v>
       </c>
       <c r="B34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" t="s">
         <v>125</v>
       </c>
-      <c r="C34" t="s">
-        <v>126</v>
-      </c>
       <c r="D34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E34" t="s">
         <v>3</v>
@@ -3247,36 +3478,39 @@
         <v>18</v>
       </c>
       <c r="M34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N34">
         <v>1</v>
       </c>
+      <c r="O34" t="s">
+        <v>285</v>
+      </c>
       <c r="P34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R34" t="s">
+        <v>241</v>
+      </c>
+      <c r="S34" t="s">
         <v>242</v>
       </c>
-      <c r="S34" t="s">
-        <v>243</v>
-      </c>
       <c r="T34" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>52</v>
       </c>
       <c r="B35" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" t="s">
         <v>128</v>
-      </c>
-      <c r="C35" t="s">
-        <v>129</v>
       </c>
       <c r="D35" t="s">
         <v>51</v>
@@ -3306,36 +3540,42 @@
         <v>18</v>
       </c>
       <c r="M35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N35">
         <v>0.55000000000000004</v>
       </c>
+      <c r="O35" t="s">
+        <v>285</v>
+      </c>
       <c r="P35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R35" t="s">
+        <v>243</v>
+      </c>
+      <c r="S35" t="s">
         <v>244</v>
       </c>
-      <c r="S35" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20">
+      <c r="T35" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>53</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" t="s">
         <v>131</v>
-      </c>
-      <c r="D36" t="s">
-        <v>132</v>
       </c>
       <c r="E36" t="s">
         <v>55</v>
@@ -3362,30 +3602,39 @@
         <v>16</v>
       </c>
       <c r="M36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N36">
         <v>0.90000000000000013</v>
       </c>
+      <c r="O36" t="s">
+        <v>285</v>
+      </c>
       <c r="P36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q36" t="s">
         <v>56</v>
       </c>
+      <c r="R36" t="s">
+        <v>285</v>
+      </c>
       <c r="S36" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20">
+        <v>132</v>
+      </c>
+      <c r="T36" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>54</v>
       </c>
       <c r="B37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" t="s">
         <v>134</v>
-      </c>
-      <c r="C37" t="s">
-        <v>135</v>
       </c>
       <c r="D37" t="s">
         <v>71</v>
@@ -3394,7 +3643,7 @@
         <v>20</v>
       </c>
       <c r="F37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -3415,27 +3664,42 @@
         <v>16</v>
       </c>
       <c r="M37" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="N37" t="s">
+        <v>285</v>
+      </c>
+      <c r="O37" t="s">
+        <v>285</v>
       </c>
       <c r="P37" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>285</v>
+      </c>
+      <c r="R37" t="s">
         <v>137</v>
       </c>
-      <c r="R37" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20">
+      <c r="S37" t="s">
+        <v>285</v>
+      </c>
+      <c r="T37" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>55</v>
       </c>
       <c r="B38" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" t="s">
         <v>139</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>140</v>
-      </c>
-      <c r="D38" t="s">
-        <v>141</v>
       </c>
       <c r="E38" t="s">
         <v>3</v>
@@ -3462,7 +3726,7 @@
         <v>16</v>
       </c>
       <c r="M38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N38">
         <v>1</v>
@@ -3471,27 +3735,33 @@
         <v>52</v>
       </c>
       <c r="P38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q38" t="s">
         <v>13</v>
       </c>
+      <c r="R38" t="s">
+        <v>285</v>
+      </c>
+      <c r="S38" t="s">
+        <v>285</v>
+      </c>
       <c r="T38" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>56</v>
       </c>
       <c r="B39" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" t="s">
         <v>143</v>
       </c>
-      <c r="C39" t="s">
-        <v>144</v>
-      </c>
       <c r="D39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E39" t="s">
         <v>3</v>
@@ -3518,7 +3788,7 @@
         <v>16</v>
       </c>
       <c r="M39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N39">
         <v>0.15000000000000002</v>
@@ -3527,33 +3797,33 @@
         <v>52</v>
       </c>
       <c r="P39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q39" t="s">
         <v>13</v>
       </c>
       <c r="R39" t="s">
+        <v>245</v>
+      </c>
+      <c r="S39" t="s">
         <v>246</v>
       </c>
-      <c r="S39" t="s">
-        <v>247</v>
-      </c>
       <c r="T39" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>57</v>
       </c>
       <c r="B40" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" t="s">
         <v>146</v>
       </c>
-      <c r="C40" t="s">
-        <v>147</v>
-      </c>
       <c r="D40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E40" t="s">
         <v>3</v>
@@ -3580,7 +3850,7 @@
         <v>16</v>
       </c>
       <c r="M40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N40">
         <v>0.55000000000000004</v>
@@ -3589,33 +3859,33 @@
         <v>52</v>
       </c>
       <c r="P40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q40" t="s">
         <v>13</v>
       </c>
       <c r="R40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="S40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T40" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>58</v>
       </c>
       <c r="B41" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" t="s">
         <v>149</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>150</v>
-      </c>
-      <c r="D41" t="s">
-        <v>151</v>
       </c>
       <c r="E41" t="s">
         <v>3</v>
@@ -3642,33 +3912,39 @@
         <v>14</v>
       </c>
       <c r="M41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N41">
         <v>0.90000000000000013</v>
       </c>
+      <c r="O41" t="s">
+        <v>285</v>
+      </c>
       <c r="P41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q41" t="s">
         <v>13</v>
       </c>
       <c r="R41" t="s">
+        <v>248</v>
+      </c>
+      <c r="S41" t="s">
         <v>249</v>
       </c>
-      <c r="S41" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20">
+      <c r="T41" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>59</v>
       </c>
       <c r="B42" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" t="s">
         <v>152</v>
-      </c>
-      <c r="C42" t="s">
-        <v>153</v>
       </c>
       <c r="D42" t="s">
         <v>71</v>
@@ -3677,7 +3953,7 @@
         <v>20</v>
       </c>
       <c r="F42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -3698,33 +3974,48 @@
         <v>14</v>
       </c>
       <c r="M42" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="N42" t="s">
+        <v>285</v>
+      </c>
+      <c r="O42" t="s">
+        <v>285</v>
       </c>
       <c r="P42" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>285</v>
+      </c>
+      <c r="R42" t="s">
         <v>137</v>
       </c>
-      <c r="R42" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20">
+      <c r="S42" t="s">
+        <v>285</v>
+      </c>
+      <c r="T42" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>62</v>
       </c>
       <c r="B43" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" t="s">
         <v>154</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>155</v>
-      </c>
-      <c r="D43" t="s">
-        <v>156</v>
       </c>
       <c r="E43" t="s">
         <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -3745,27 +4036,39 @@
         <v>10</v>
       </c>
       <c r="M43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N43">
         <v>0.05</v>
       </c>
+      <c r="O43" t="s">
+        <v>285</v>
+      </c>
       <c r="P43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q43" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20">
+        <v>157</v>
+      </c>
+      <c r="R43" t="s">
+        <v>285</v>
+      </c>
+      <c r="S43" t="s">
+        <v>285</v>
+      </c>
+      <c r="T43" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>67</v>
       </c>
       <c r="B44" t="s">
+        <v>158</v>
+      </c>
+      <c r="C44" t="s">
         <v>159</v>
-      </c>
-      <c r="C44" t="s">
-        <v>160</v>
       </c>
       <c r="D44" t="s">
         <v>71</v>
@@ -3774,7 +4077,7 @@
         <v>20</v>
       </c>
       <c r="F44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -3795,24 +4098,39 @@
         <v>8</v>
       </c>
       <c r="M44" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="N44" t="s">
+        <v>285</v>
+      </c>
+      <c r="O44" t="s">
+        <v>285</v>
       </c>
       <c r="P44" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>285</v>
+      </c>
+      <c r="R44" t="s">
         <v>137</v>
       </c>
-      <c r="R44" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20">
+      <c r="S44" t="s">
+        <v>285</v>
+      </c>
+      <c r="T44" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>70</v>
       </c>
       <c r="B45" t="s">
+        <v>160</v>
+      </c>
+      <c r="C45" t="s">
         <v>161</v>
-      </c>
-      <c r="C45" t="s">
-        <v>162</v>
       </c>
       <c r="D45" t="s">
         <v>42</v>
@@ -3821,7 +4139,7 @@
         <v>20</v>
       </c>
       <c r="F45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -3842,27 +4160,42 @@
         <v>6</v>
       </c>
       <c r="M45" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="N45" t="s">
+        <v>285</v>
+      </c>
+      <c r="O45" t="s">
+        <v>285</v>
       </c>
       <c r="P45" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>285</v>
+      </c>
+      <c r="R45" t="s">
         <v>137</v>
       </c>
-      <c r="R45" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20">
+      <c r="S45" t="s">
+        <v>285</v>
+      </c>
+      <c r="T45" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>74</v>
       </c>
       <c r="B46" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" t="s">
         <v>163</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>164</v>
-      </c>
-      <c r="D46" t="s">
-        <v>165</v>
       </c>
       <c r="E46" t="s">
         <v>55</v>
@@ -3889,7 +4222,7 @@
         <v>6</v>
       </c>
       <c r="M46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N46">
         <v>0.35000000000000003</v>
@@ -3898,33 +4231,33 @@
         <v>52</v>
       </c>
       <c r="P46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R46" t="s">
+        <v>250</v>
+      </c>
+      <c r="S46" t="s">
         <v>251</v>
       </c>
-      <c r="S46" t="s">
-        <v>252</v>
-      </c>
       <c r="T46" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>78</v>
       </c>
       <c r="B47" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47" t="s">
         <v>167</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>168</v>
-      </c>
-      <c r="D47" t="s">
-        <v>169</v>
       </c>
       <c r="E47" t="s">
         <v>20</v>
@@ -3932,37 +4265,61 @@
       <c r="F47" t="s">
         <v>37</v>
       </c>
+      <c r="G47" t="s">
+        <v>285</v>
+      </c>
+      <c r="H47" t="s">
+        <v>285</v>
+      </c>
+      <c r="I47" t="s">
+        <v>285</v>
+      </c>
+      <c r="J47" t="s">
+        <v>285</v>
+      </c>
+      <c r="K47" t="s">
+        <v>285</v>
+      </c>
+      <c r="L47" t="s">
+        <v>285</v>
+      </c>
       <c r="M47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N47">
         <v>0.05</v>
       </c>
+      <c r="O47" t="s">
+        <v>285</v>
+      </c>
       <c r="P47" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q47" t="s">
         <v>13</v>
       </c>
       <c r="R47" t="s">
+        <v>252</v>
+      </c>
+      <c r="S47" t="s">
         <v>253</v>
       </c>
-      <c r="S47" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20">
+      <c r="T47" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>79</v>
       </c>
       <c r="B48" t="s">
+        <v>169</v>
+      </c>
+      <c r="C48" t="s">
         <v>170</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>171</v>
-      </c>
-      <c r="D48" t="s">
-        <v>172</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
@@ -3989,7 +4346,7 @@
         <v>6</v>
       </c>
       <c r="M48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N48">
         <v>0.15000000000000002</v>
@@ -3998,33 +4355,33 @@
         <v>52</v>
       </c>
       <c r="P48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q48" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R48" t="s">
+        <v>254</v>
+      </c>
+      <c r="S48" t="s">
         <v>255</v>
       </c>
-      <c r="S48" t="s">
-        <v>256</v>
-      </c>
       <c r="T48" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>83</v>
       </c>
       <c r="B49" t="s">
+        <v>173</v>
+      </c>
+      <c r="C49" t="s">
         <v>174</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>175</v>
-      </c>
-      <c r="D49" t="s">
-        <v>176</v>
       </c>
       <c r="E49" t="s">
         <v>3</v>
@@ -4032,37 +4389,61 @@
       <c r="F49" t="s">
         <v>37</v>
       </c>
+      <c r="G49" t="s">
+        <v>285</v>
+      </c>
+      <c r="H49" t="s">
+        <v>285</v>
+      </c>
+      <c r="I49" t="s">
+        <v>285</v>
+      </c>
+      <c r="J49" t="s">
+        <v>285</v>
+      </c>
+      <c r="K49" t="s">
+        <v>285</v>
+      </c>
+      <c r="L49" t="s">
+        <v>285</v>
+      </c>
       <c r="M49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N49">
         <v>0.35</v>
       </c>
+      <c r="O49" t="s">
+        <v>285</v>
+      </c>
       <c r="P49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R49" t="s">
+        <v>256</v>
+      </c>
+      <c r="S49" t="s">
         <v>257</v>
       </c>
-      <c r="S49" t="s">
-        <v>258</v>
-      </c>
       <c r="T49" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>84</v>
       </c>
       <c r="B50" t="s">
+        <v>177</v>
+      </c>
+      <c r="C50" t="s">
+        <v>285</v>
+      </c>
+      <c r="D50" t="s">
         <v>178</v>
-      </c>
-      <c r="D50" t="s">
-        <v>179</v>
       </c>
       <c r="E50" t="s">
         <v>3</v>
@@ -4070,31 +4451,61 @@
       <c r="F50" t="s">
         <v>4</v>
       </c>
+      <c r="G50" t="s">
+        <v>285</v>
+      </c>
+      <c r="H50" t="s">
+        <v>285</v>
+      </c>
+      <c r="I50" t="s">
+        <v>285</v>
+      </c>
+      <c r="J50" t="s">
+        <v>285</v>
+      </c>
+      <c r="K50" t="s">
+        <v>285</v>
+      </c>
+      <c r="L50" t="s">
+        <v>285</v>
+      </c>
       <c r="M50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N50">
         <v>0.9</v>
       </c>
+      <c r="O50" t="s">
+        <v>285</v>
+      </c>
       <c r="P50" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q50" t="s">
         <v>180</v>
       </c>
-      <c r="Q50" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20">
+      <c r="R50" t="s">
+        <v>285</v>
+      </c>
+      <c r="S50" t="s">
+        <v>285</v>
+      </c>
+      <c r="T50" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>85</v>
       </c>
       <c r="B51" t="s">
+        <v>181</v>
+      </c>
+      <c r="C51" t="s">
         <v>182</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>183</v>
-      </c>
-      <c r="D51" t="s">
-        <v>184</v>
       </c>
       <c r="E51" t="s">
         <v>20</v>
@@ -4102,37 +4513,61 @@
       <c r="F51" t="s">
         <v>37</v>
       </c>
+      <c r="G51" t="s">
+        <v>285</v>
+      </c>
+      <c r="H51" t="s">
+        <v>285</v>
+      </c>
+      <c r="I51" t="s">
+        <v>285</v>
+      </c>
+      <c r="J51" t="s">
+        <v>285</v>
+      </c>
+      <c r="K51" t="s">
+        <v>285</v>
+      </c>
+      <c r="L51" t="s">
+        <v>285</v>
+      </c>
       <c r="M51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N51">
         <v>0.25</v>
       </c>
+      <c r="O51" t="s">
+        <v>285</v>
+      </c>
       <c r="P51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q51" t="s">
+        <v>184</v>
+      </c>
+      <c r="R51" t="s">
+        <v>258</v>
+      </c>
+      <c r="S51" t="s">
+        <v>259</v>
+      </c>
+      <c r="T51" t="s">
         <v>185</v>
       </c>
-      <c r="R51" t="s">
-        <v>259</v>
-      </c>
-      <c r="S51" t="s">
-        <v>260</v>
-      </c>
-      <c r="T51" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20">
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>86</v>
       </c>
       <c r="B52" t="s">
+        <v>186</v>
+      </c>
+      <c r="C52" t="s">
+        <v>285</v>
+      </c>
+      <c r="D52" t="s">
         <v>187</v>
-      </c>
-      <c r="D52" t="s">
-        <v>188</v>
       </c>
       <c r="E52" t="s">
         <v>20</v>
@@ -4140,37 +4575,58 @@
       <c r="F52" t="s">
         <v>37</v>
       </c>
+      <c r="G52" t="s">
+        <v>285</v>
+      </c>
+      <c r="H52" t="s">
+        <v>285</v>
+      </c>
+      <c r="I52" t="s">
+        <v>285</v>
+      </c>
+      <c r="J52" t="s">
+        <v>285</v>
+      </c>
+      <c r="K52" t="s">
+        <v>285</v>
+      </c>
+      <c r="L52" t="s">
+        <v>285</v>
+      </c>
       <c r="M52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N52">
         <v>0.45</v>
       </c>
+      <c r="O52" t="s">
+        <v>285</v>
+      </c>
       <c r="P52" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q52" t="s">
         <v>13</v>
       </c>
       <c r="R52" t="s">
+        <v>260</v>
+      </c>
+      <c r="S52" t="s">
         <v>261</v>
       </c>
-      <c r="S52" t="s">
-        <v>262</v>
-      </c>
       <c r="T52" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>87</v>
       </c>
       <c r="B53" t="s">
+        <v>189</v>
+      </c>
+      <c r="C53" t="s">
         <v>190</v>
-      </c>
-      <c r="C53" t="s">
-        <v>191</v>
       </c>
       <c r="D53" t="s">
         <v>42</v>
@@ -4200,7 +4656,7 @@
         <v>19</v>
       </c>
       <c r="M53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N53">
         <v>0.1</v>
@@ -4209,59 +4665,92 @@
         <v>6</v>
       </c>
       <c r="P53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q53" t="s">
+        <v>191</v>
+      </c>
+      <c r="R53" t="s">
+        <v>262</v>
+      </c>
+      <c r="S53" t="s">
+        <v>263</v>
+      </c>
+      <c r="T53" t="s">
         <v>192</v>
       </c>
-      <c r="R53" t="s">
-        <v>263</v>
-      </c>
-      <c r="S53" t="s">
-        <v>264</v>
-      </c>
-      <c r="T53" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20">
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>88</v>
       </c>
       <c r="B54" t="s">
+        <v>193</v>
+      </c>
+      <c r="C54" t="s">
         <v>194</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
+        <v>183</v>
+      </c>
+      <c r="E54" t="s">
         <v>195</v>
       </c>
-      <c r="D54" t="s">
-        <v>184</v>
-      </c>
-      <c r="E54" t="s">
-        <v>196</v>
-      </c>
       <c r="F54" t="s">
-        <v>196</v>
+        <v>195</v>
+      </c>
+      <c r="G54" t="s">
+        <v>285</v>
+      </c>
+      <c r="H54" t="s">
+        <v>285</v>
+      </c>
+      <c r="I54" t="s">
+        <v>285</v>
+      </c>
+      <c r="J54" t="s">
+        <v>285</v>
+      </c>
+      <c r="K54" t="s">
+        <v>285</v>
+      </c>
+      <c r="L54" t="s">
+        <v>285</v>
       </c>
       <c r="M54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N54">
         <v>0</v>
       </c>
+      <c r="O54" t="s">
+        <v>285</v>
+      </c>
+      <c r="P54" t="s">
+        <v>285</v>
+      </c>
       <c r="Q54" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20">
+        <v>184</v>
+      </c>
+      <c r="R54" t="s">
+        <v>285</v>
+      </c>
+      <c r="S54" t="s">
+        <v>285</v>
+      </c>
+      <c r="T54" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>89</v>
       </c>
       <c r="B55" t="s">
+        <v>196</v>
+      </c>
+      <c r="C55" t="s">
         <v>197</v>
-      </c>
-      <c r="C55" t="s">
-        <v>198</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
@@ -4291,7 +4780,7 @@
         <v>21</v>
       </c>
       <c r="M55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N55">
         <v>0.15</v>
@@ -4300,19 +4789,19 @@
         <v>52</v>
       </c>
       <c r="P55" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q55" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R55" t="s">
+        <v>264</v>
+      </c>
+      <c r="S55" t="s">
         <v>265</v>
       </c>
-      <c r="S55" t="s">
-        <v>266</v>
-      </c>
       <c r="T55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -4343,5 +4832,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se envía a prod vía railway
</commit_message>
<xml_diff>
--- a/ProyectosEjemplo.xlsx
+++ b/ProyectosEjemplo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulloa\Desktop\Proyectos Desarrollo\ChatBotXOne\AppChatBotXOne - Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB48D99A-473A-4181-A17D-4269CFD6EDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7B5B22-7224-4738-B13F-17418E013B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15AA1E02-0B31-4ADF-81E4-BED79850A1EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="286">
   <si>
     <t>TABLA DE DESCUENTOS SEGÚN VOLUMEN DE COMPRA</t>
   </si>
@@ -285,9 +285,6 @@
   </si>
   <si>
     <t>AUTOMATIZACION DE MINIMO BODEGA CENTRAL</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>MARIA JOSE POZO</t>
@@ -916,6 +913,9 @@
   </si>
   <si>
     <t>FECHA ESTIMADA DEL PRIMER PILOTO</t>
+  </si>
+  <si>
+    <t>PENDIENTE</t>
   </si>
 </sst>
 </file>
@@ -1371,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0256956B-D125-4E51-96AC-4BDE41623DD8}">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1386,62 +1386,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="34.5" customHeight="1">
+      <c r="A1" t="s">
+        <v>285</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -1491,16 +1494,16 @@
         <v>6</v>
       </c>
       <c r="P2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q2" t="s">
         <v>7</v>
       </c>
       <c r="R2" t="s">
+        <v>198</v>
+      </c>
+      <c r="S2" t="s">
         <v>199</v>
-      </c>
-      <c r="S2" t="s">
-        <v>200</v>
       </c>
       <c r="T2" t="s">
         <v>8</v>
@@ -1553,16 +1556,16 @@
         <v>6</v>
       </c>
       <c r="P3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q3" t="s">
         <v>13</v>
       </c>
       <c r="R3" t="s">
+        <v>200</v>
+      </c>
+      <c r="S3" t="s">
         <v>201</v>
-      </c>
-      <c r="S3" t="s">
-        <v>202</v>
       </c>
       <c r="T3" t="s">
         <v>14</v>
@@ -1615,16 +1618,16 @@
         <v>6</v>
       </c>
       <c r="P4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q4" t="s">
         <v>13</v>
       </c>
       <c r="R4" t="s">
+        <v>202</v>
+      </c>
+      <c r="S4" t="s">
         <v>203</v>
-      </c>
-      <c r="S4" t="s">
-        <v>204</v>
       </c>
       <c r="T4" t="s">
         <v>17</v>
@@ -1635,7 +1638,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -1677,16 +1680,19 @@
         <v>21</v>
       </c>
       <c r="P5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q5" t="s">
         <v>22</v>
       </c>
       <c r="R5" t="s">
+        <v>206</v>
+      </c>
+      <c r="S5" t="s">
         <v>207</v>
       </c>
-      <c r="S5" t="s">
-        <v>208</v>
+      <c r="T5" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -1736,16 +1742,16 @@
         <v>21</v>
       </c>
       <c r="P6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q6" t="s">
         <v>25</v>
       </c>
       <c r="R6" t="s">
+        <v>208</v>
+      </c>
+      <c r="S6" t="s">
         <v>209</v>
-      </c>
-      <c r="S6" t="s">
-        <v>210</v>
       </c>
       <c r="T6" t="s">
         <v>26</v>
@@ -1798,16 +1804,16 @@
         <v>31</v>
       </c>
       <c r="P7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q7" t="s">
         <v>32</v>
       </c>
       <c r="R7" t="s">
+        <v>210</v>
+      </c>
+      <c r="S7" t="s">
         <v>211</v>
-      </c>
-      <c r="S7" t="s">
-        <v>212</v>
       </c>
       <c r="T7" t="s">
         <v>33</v>
@@ -1860,16 +1866,16 @@
         <v>31</v>
       </c>
       <c r="P8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q8" t="s">
         <v>38</v>
       </c>
       <c r="R8" t="s">
+        <v>212</v>
+      </c>
+      <c r="S8" t="s">
         <v>213</v>
-      </c>
-      <c r="S8" t="s">
-        <v>214</v>
       </c>
       <c r="T8" t="s">
         <v>39</v>
@@ -1922,10 +1928,19 @@
         <v>6</v>
       </c>
       <c r="P9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q9" t="s">
         <v>44</v>
+      </c>
+      <c r="R9" t="s">
+        <v>285</v>
+      </c>
+      <c r="S9" t="s">
+        <v>285</v>
+      </c>
+      <c r="T9" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1975,16 +1990,19 @@
         <v>31</v>
       </c>
       <c r="P10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q10" t="s">
         <v>32</v>
       </c>
       <c r="R10" t="s">
+        <v>214</v>
+      </c>
+      <c r="S10" t="s">
         <v>215</v>
       </c>
-      <c r="S10" t="s">
-        <v>216</v>
+      <c r="T10" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -2034,16 +2052,19 @@
         <v>31</v>
       </c>
       <c r="P11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q11" t="s">
         <v>32</v>
       </c>
       <c r="R11" t="s">
+        <v>216</v>
+      </c>
+      <c r="S11" t="s">
         <v>217</v>
       </c>
-      <c r="S11" t="s">
-        <v>218</v>
+      <c r="T11" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -2093,10 +2114,19 @@
         <v>52</v>
       </c>
       <c r="P12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q12" t="s">
         <v>13</v>
+      </c>
+      <c r="R12" t="s">
+        <v>285</v>
+      </c>
+      <c r="S12" t="s">
+        <v>285</v>
+      </c>
+      <c r="T12" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -2146,16 +2176,19 @@
         <v>52</v>
       </c>
       <c r="P13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q13" t="s">
         <v>56</v>
       </c>
       <c r="R13" t="s">
+        <v>218</v>
+      </c>
+      <c r="S13" t="s">
         <v>219</v>
       </c>
-      <c r="S13" t="s">
-        <v>220</v>
+      <c r="T13" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -2205,10 +2238,19 @@
         <v>52</v>
       </c>
       <c r="P14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q14" t="s">
         <v>56</v>
+      </c>
+      <c r="R14" t="s">
+        <v>285</v>
+      </c>
+      <c r="S14" t="s">
+        <v>285</v>
+      </c>
+      <c r="T14" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -2258,10 +2300,19 @@
         <v>52</v>
       </c>
       <c r="P15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q15" t="s">
         <v>56</v>
+      </c>
+      <c r="R15" t="s">
+        <v>285</v>
+      </c>
+      <c r="S15" t="s">
+        <v>285</v>
+      </c>
+      <c r="T15" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -2311,10 +2362,19 @@
         <v>52</v>
       </c>
       <c r="P16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q16" t="s">
         <v>56</v>
+      </c>
+      <c r="R16" t="s">
+        <v>285</v>
+      </c>
+      <c r="S16" t="s">
+        <v>285</v>
+      </c>
+      <c r="T16" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -2364,16 +2424,16 @@
         <v>66</v>
       </c>
       <c r="P17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q17" t="s">
         <v>67</v>
       </c>
       <c r="R17" t="s">
+        <v>220</v>
+      </c>
+      <c r="S17" t="s">
         <v>221</v>
-      </c>
-      <c r="S17" t="s">
-        <v>222</v>
       </c>
       <c r="T17" t="s">
         <v>68</v>
@@ -2426,16 +2486,16 @@
         <v>6</v>
       </c>
       <c r="P18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q18" t="s">
         <v>7</v>
       </c>
       <c r="R18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="S18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T18" t="s">
         <v>72</v>
@@ -2488,13 +2548,16 @@
         <v>6</v>
       </c>
       <c r="P19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q19" t="s">
         <v>7</v>
       </c>
       <c r="R19" t="s">
-        <v>224</v>
+        <v>223</v>
+      </c>
+      <c r="S19" t="s">
+        <v>285</v>
       </c>
       <c r="T19" t="s">
         <v>75</v>
@@ -2547,13 +2610,19 @@
         <v>52</v>
       </c>
       <c r="P20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q20" t="s">
         <v>79</v>
       </c>
       <c r="R20" t="s">
         <v>80</v>
+      </c>
+      <c r="S20" t="s">
+        <v>285</v>
+      </c>
+      <c r="T20" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -2564,10 +2633,10 @@
         <v>81</v>
       </c>
       <c r="C21" t="s">
+        <v>285</v>
+      </c>
+      <c r="D21" t="s">
         <v>82</v>
-      </c>
-      <c r="D21" t="s">
-        <v>83</v>
       </c>
       <c r="E21" t="s">
         <v>55</v>
@@ -2599,11 +2668,23 @@
       <c r="N21">
         <v>0.35</v>
       </c>
+      <c r="O21" t="s">
+        <v>285</v>
+      </c>
       <c r="P21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q21" t="s">
         <v>56</v>
+      </c>
+      <c r="R21" t="s">
+        <v>285</v>
+      </c>
+      <c r="S21" t="s">
+        <v>285</v>
+      </c>
+      <c r="T21" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -2611,10 +2692,10 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" t="s">
         <v>84</v>
-      </c>
-      <c r="C22" t="s">
-        <v>85</v>
       </c>
       <c r="D22" t="s">
         <v>54</v>
@@ -2653,19 +2734,19 @@
         <v>52</v>
       </c>
       <c r="P22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q22" t="s">
         <v>56</v>
       </c>
       <c r="R22" t="s">
+        <v>224</v>
+      </c>
+      <c r="S22" t="s">
         <v>225</v>
       </c>
-      <c r="S22" t="s">
-        <v>226</v>
-      </c>
       <c r="T22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -2673,19 +2754,19 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" t="s">
         <v>87</v>
-      </c>
-      <c r="C23" t="s">
-        <v>88</v>
       </c>
       <c r="D23" t="s">
         <v>78</v>
       </c>
       <c r="E23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" t="s">
         <v>89</v>
-      </c>
-      <c r="F23" t="s">
-        <v>90</v>
       </c>
       <c r="G23">
         <v>8</v>
@@ -2715,10 +2796,19 @@
         <v>52</v>
       </c>
       <c r="P23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q23" t="s">
         <v>79</v>
+      </c>
+      <c r="R23" t="s">
+        <v>285</v>
+      </c>
+      <c r="S23" t="s">
+        <v>285</v>
+      </c>
+      <c r="T23" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:20">
@@ -2726,7 +2816,10 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="C24" t="s">
+        <v>285</v>
       </c>
       <c r="D24" t="s">
         <v>51</v>
@@ -2737,6 +2830,21 @@
       <c r="F24" t="s">
         <v>30</v>
       </c>
+      <c r="G24" t="s">
+        <v>285</v>
+      </c>
+      <c r="H24" t="s">
+        <v>285</v>
+      </c>
+      <c r="I24" t="s">
+        <v>285</v>
+      </c>
+      <c r="J24" t="s">
+        <v>285</v>
+      </c>
+      <c r="K24" t="s">
+        <v>285</v>
+      </c>
       <c r="L24">
         <v>0</v>
       </c>
@@ -2746,17 +2854,20 @@
       <c r="N24">
         <v>0.90000000000000013</v>
       </c>
+      <c r="O24" t="s">
+        <v>285</v>
+      </c>
       <c r="P24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q24" t="s">
         <v>56</v>
       </c>
       <c r="R24" t="s">
+        <v>226</v>
+      </c>
+      <c r="S24" t="s">
         <v>227</v>
-      </c>
-      <c r="S24" t="s">
-        <v>228</v>
       </c>
       <c r="T24" t="s">
         <v>33</v>
@@ -2767,10 +2878,13 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
+        <v>285</v>
+      </c>
+      <c r="D25" t="s">
         <v>93</v>
-      </c>
-      <c r="D25" t="s">
-        <v>94</v>
       </c>
       <c r="E25" t="s">
         <v>55</v>
@@ -2778,6 +2892,21 @@
       <c r="F25" t="s">
         <v>30</v>
       </c>
+      <c r="G25" t="s">
+        <v>285</v>
+      </c>
+      <c r="H25" t="s">
+        <v>285</v>
+      </c>
+      <c r="I25" t="s">
+        <v>285</v>
+      </c>
+      <c r="J25" t="s">
+        <v>285</v>
+      </c>
+      <c r="K25" t="s">
+        <v>285</v>
+      </c>
       <c r="L25">
         <v>0</v>
       </c>
@@ -2787,17 +2916,20 @@
       <c r="N25">
         <v>0.84999999999999987</v>
       </c>
+      <c r="O25" t="s">
+        <v>285</v>
+      </c>
       <c r="P25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q25" t="s">
         <v>56</v>
       </c>
       <c r="R25" t="s">
+        <v>228</v>
+      </c>
+      <c r="S25" t="s">
         <v>229</v>
-      </c>
-      <c r="S25" t="s">
-        <v>230</v>
       </c>
       <c r="T25" t="s">
         <v>33</v>
@@ -2808,7 +2940,10 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="C26" t="s">
+        <v>285</v>
       </c>
       <c r="D26" t="s">
         <v>51</v>
@@ -2819,6 +2954,21 @@
       <c r="F26" t="s">
         <v>30</v>
       </c>
+      <c r="G26" t="s">
+        <v>285</v>
+      </c>
+      <c r="H26" t="s">
+        <v>285</v>
+      </c>
+      <c r="I26" t="s">
+        <v>285</v>
+      </c>
+      <c r="J26" t="s">
+        <v>285</v>
+      </c>
+      <c r="K26" t="s">
+        <v>285</v>
+      </c>
       <c r="L26">
         <v>0</v>
       </c>
@@ -2828,11 +2978,23 @@
       <c r="N26">
         <v>1</v>
       </c>
+      <c r="O26" t="s">
+        <v>285</v>
+      </c>
       <c r="P26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q26" t="s">
         <v>56</v>
+      </c>
+      <c r="R26" t="s">
+        <v>285</v>
+      </c>
+      <c r="S26" t="s">
+        <v>285</v>
+      </c>
+      <c r="T26" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="27" spans="1:20">
@@ -2840,13 +3002,13 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" t="s">
         <v>96</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>97</v>
-      </c>
-      <c r="D27" t="s">
-        <v>98</v>
       </c>
       <c r="E27" t="s">
         <v>20</v>
@@ -2882,19 +3044,19 @@
         <v>21</v>
       </c>
       <c r="P27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q27" t="s">
+        <v>98</v>
+      </c>
+      <c r="R27" t="s">
+        <v>230</v>
+      </c>
+      <c r="S27" t="s">
+        <v>231</v>
+      </c>
+      <c r="T27" t="s">
         <v>99</v>
-      </c>
-      <c r="R27" t="s">
-        <v>231</v>
-      </c>
-      <c r="S27" t="s">
-        <v>232</v>
-      </c>
-      <c r="T27" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:20">
@@ -2902,13 +3064,13 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" t="s">
         <v>101</v>
       </c>
-      <c r="C28" t="s">
-        <v>102</v>
-      </c>
       <c r="D28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E28" t="s">
         <v>20</v>
@@ -2916,6 +3078,21 @@
       <c r="F28" t="s">
         <v>37</v>
       </c>
+      <c r="G28" t="s">
+        <v>285</v>
+      </c>
+      <c r="H28" t="s">
+        <v>285</v>
+      </c>
+      <c r="I28" t="s">
+        <v>285</v>
+      </c>
+      <c r="J28" t="s">
+        <v>285</v>
+      </c>
+      <c r="K28" t="s">
+        <v>285</v>
+      </c>
       <c r="L28">
         <v>0</v>
       </c>
@@ -2925,20 +3102,23 @@
       <c r="N28">
         <v>0.55000000000000004</v>
       </c>
+      <c r="O28" t="s">
+        <v>285</v>
+      </c>
       <c r="P28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q28" t="s">
         <v>13</v>
       </c>
       <c r="R28" t="s">
+        <v>232</v>
+      </c>
+      <c r="S28" t="s">
         <v>233</v>
       </c>
-      <c r="S28" t="s">
-        <v>234</v>
-      </c>
       <c r="T28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:20">
@@ -2946,13 +3126,13 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" t="s">
         <v>104</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>105</v>
-      </c>
-      <c r="D29" t="s">
-        <v>106</v>
       </c>
       <c r="E29" t="s">
         <v>3</v>
@@ -2960,6 +3140,21 @@
       <c r="F29" t="s">
         <v>4</v>
       </c>
+      <c r="G29" t="s">
+        <v>285</v>
+      </c>
+      <c r="H29" t="s">
+        <v>285</v>
+      </c>
+      <c r="I29" t="s">
+        <v>285</v>
+      </c>
+      <c r="J29" t="s">
+        <v>285</v>
+      </c>
+      <c r="K29" t="s">
+        <v>285</v>
+      </c>
       <c r="L29">
         <v>0</v>
       </c>
@@ -2969,17 +3164,23 @@
       <c r="N29">
         <v>0.5</v>
       </c>
+      <c r="O29" t="s">
+        <v>285</v>
+      </c>
       <c r="P29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q29" t="s">
         <v>32</v>
       </c>
       <c r="R29" t="s">
+        <v>234</v>
+      </c>
+      <c r="S29" t="s">
         <v>235</v>
       </c>
-      <c r="S29" t="s">
-        <v>236</v>
+      <c r="T29" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="30" spans="1:20">
@@ -2987,16 +3188,16 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" t="s">
         <v>107</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>108</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>109</v>
-      </c>
-      <c r="E30" t="s">
-        <v>110</v>
       </c>
       <c r="F30" t="s">
         <v>4</v>
@@ -3020,16 +3221,28 @@
         <v>30</v>
       </c>
       <c r="M30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N30">
         <v>1</v>
       </c>
+      <c r="O30" t="s">
+        <v>285</v>
+      </c>
       <c r="P30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q30" t="s">
         <v>67</v>
+      </c>
+      <c r="R30" t="s">
+        <v>285</v>
+      </c>
+      <c r="S30" t="s">
+        <v>285</v>
+      </c>
+      <c r="T30" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="31" spans="1:20">
@@ -3037,13 +3250,13 @@
         <v>37</v>
       </c>
       <c r="B31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" t="s">
         <v>113</v>
       </c>
-      <c r="C31" t="s">
-        <v>114</v>
-      </c>
       <c r="D31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E31" t="s">
         <v>3</v>
@@ -3070,25 +3283,28 @@
         <v>30</v>
       </c>
       <c r="M31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N31">
         <v>0.2</v>
       </c>
+      <c r="O31" t="s">
+        <v>285</v>
+      </c>
       <c r="P31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q31" t="s">
+        <v>114</v>
+      </c>
+      <c r="R31" t="s">
+        <v>236</v>
+      </c>
+      <c r="S31" t="s">
+        <v>237</v>
+      </c>
+      <c r="T31" t="s">
         <v>115</v>
-      </c>
-      <c r="R31" t="s">
-        <v>237</v>
-      </c>
-      <c r="S31" t="s">
-        <v>238</v>
-      </c>
-      <c r="T31" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:20">
@@ -3096,13 +3312,13 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" t="s">
         <v>117</v>
       </c>
-      <c r="C32" t="s">
-        <v>118</v>
-      </c>
       <c r="D32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E32" t="s">
         <v>3</v>
@@ -3129,25 +3345,28 @@
         <v>30</v>
       </c>
       <c r="M32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N32">
         <v>0.2</v>
       </c>
+      <c r="O32" t="s">
+        <v>285</v>
+      </c>
       <c r="P32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R32" t="s">
+        <v>238</v>
+      </c>
+      <c r="S32" t="s">
         <v>239</v>
       </c>
-      <c r="S32" t="s">
-        <v>240</v>
-      </c>
       <c r="T32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:20">
@@ -3155,13 +3374,13 @@
         <v>50</v>
       </c>
       <c r="B33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" t="s">
         <v>120</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>121</v>
-      </c>
-      <c r="D33" t="s">
-        <v>122</v>
       </c>
       <c r="E33" t="s">
         <v>3</v>
@@ -3188,25 +3407,28 @@
         <v>20</v>
       </c>
       <c r="M33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N33">
         <v>1.0000000000000002</v>
       </c>
+      <c r="O33" t="s">
+        <v>285</v>
+      </c>
       <c r="P33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q33" t="s">
+        <v>122</v>
+      </c>
+      <c r="R33" t="s">
+        <v>240</v>
+      </c>
+      <c r="S33" t="s">
+        <v>240</v>
+      </c>
+      <c r="T33" t="s">
         <v>123</v>
-      </c>
-      <c r="R33" t="s">
-        <v>241</v>
-      </c>
-      <c r="S33" t="s">
-        <v>241</v>
-      </c>
-      <c r="T33" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:20">
@@ -3214,13 +3436,13 @@
         <v>51</v>
       </c>
       <c r="B34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" t="s">
         <v>125</v>
       </c>
-      <c r="C34" t="s">
-        <v>126</v>
-      </c>
       <c r="D34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E34" t="s">
         <v>3</v>
@@ -3247,25 +3469,28 @@
         <v>18</v>
       </c>
       <c r="M34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N34">
         <v>1</v>
       </c>
+      <c r="O34" t="s">
+        <v>285</v>
+      </c>
       <c r="P34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R34" t="s">
+        <v>241</v>
+      </c>
+      <c r="S34" t="s">
         <v>242</v>
       </c>
-      <c r="S34" t="s">
-        <v>243</v>
-      </c>
       <c r="T34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:20">
@@ -3273,10 +3498,10 @@
         <v>52</v>
       </c>
       <c r="B35" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" t="s">
         <v>128</v>
-      </c>
-      <c r="C35" t="s">
-        <v>129</v>
       </c>
       <c r="D35" t="s">
         <v>51</v>
@@ -3306,22 +3531,28 @@
         <v>18</v>
       </c>
       <c r="M35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N35">
         <v>0.55000000000000004</v>
       </c>
+      <c r="O35" t="s">
+        <v>285</v>
+      </c>
       <c r="P35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R35" t="s">
+        <v>243</v>
+      </c>
+      <c r="S35" t="s">
         <v>244</v>
       </c>
-      <c r="S35" t="s">
-        <v>245</v>
+      <c r="T35" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -3329,13 +3560,13 @@
         <v>53</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" t="s">
         <v>131</v>
-      </c>
-      <c r="D36" t="s">
-        <v>132</v>
       </c>
       <c r="E36" t="s">
         <v>55</v>
@@ -3362,19 +3593,28 @@
         <v>16</v>
       </c>
       <c r="M36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N36">
         <v>0.90000000000000013</v>
       </c>
+      <c r="O36" t="s">
+        <v>285</v>
+      </c>
       <c r="P36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q36" t="s">
         <v>56</v>
       </c>
+      <c r="R36" t="s">
+        <v>285</v>
+      </c>
       <c r="S36" t="s">
-        <v>133</v>
+        <v>132</v>
+      </c>
+      <c r="T36" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="37" spans="1:20">
@@ -3382,10 +3622,10 @@
         <v>54</v>
       </c>
       <c r="B37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" t="s">
         <v>134</v>
-      </c>
-      <c r="C37" t="s">
-        <v>135</v>
       </c>
       <c r="D37" t="s">
         <v>71</v>
@@ -3394,7 +3634,7 @@
         <v>20</v>
       </c>
       <c r="F37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -3415,13 +3655,28 @@
         <v>16</v>
       </c>
       <c r="M37" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="N37" t="s">
+        <v>285</v>
+      </c>
+      <c r="O37" t="s">
+        <v>285</v>
       </c>
       <c r="P37" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>285</v>
+      </c>
+      <c r="R37" t="s">
         <v>137</v>
       </c>
-      <c r="R37" t="s">
-        <v>138</v>
+      <c r="S37" t="s">
+        <v>285</v>
+      </c>
+      <c r="T37" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="38" spans="1:20">
@@ -3429,13 +3684,13 @@
         <v>55</v>
       </c>
       <c r="B38" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" t="s">
         <v>139</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>140</v>
-      </c>
-      <c r="D38" t="s">
-        <v>141</v>
       </c>
       <c r="E38" t="s">
         <v>3</v>
@@ -3462,7 +3717,7 @@
         <v>16</v>
       </c>
       <c r="M38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N38">
         <v>1</v>
@@ -3471,13 +3726,19 @@
         <v>52</v>
       </c>
       <c r="P38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q38" t="s">
         <v>13</v>
       </c>
+      <c r="R38" t="s">
+        <v>285</v>
+      </c>
+      <c r="S38" t="s">
+        <v>285</v>
+      </c>
       <c r="T38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:20">
@@ -3485,13 +3746,13 @@
         <v>56</v>
       </c>
       <c r="B39" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" t="s">
         <v>143</v>
       </c>
-      <c r="C39" t="s">
-        <v>144</v>
-      </c>
       <c r="D39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E39" t="s">
         <v>3</v>
@@ -3518,7 +3779,7 @@
         <v>16</v>
       </c>
       <c r="M39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N39">
         <v>0.15000000000000002</v>
@@ -3527,19 +3788,19 @@
         <v>52</v>
       </c>
       <c r="P39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q39" t="s">
         <v>13</v>
       </c>
       <c r="R39" t="s">
+        <v>245</v>
+      </c>
+      <c r="S39" t="s">
         <v>246</v>
       </c>
-      <c r="S39" t="s">
-        <v>247</v>
-      </c>
       <c r="T39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:20">
@@ -3547,13 +3808,13 @@
         <v>57</v>
       </c>
       <c r="B40" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" t="s">
         <v>146</v>
       </c>
-      <c r="C40" t="s">
-        <v>147</v>
-      </c>
       <c r="D40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E40" t="s">
         <v>3</v>
@@ -3580,7 +3841,7 @@
         <v>16</v>
       </c>
       <c r="M40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N40">
         <v>0.55000000000000004</v>
@@ -3589,19 +3850,19 @@
         <v>52</v>
       </c>
       <c r="P40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q40" t="s">
         <v>13</v>
       </c>
       <c r="R40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="S40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:20">
@@ -3609,13 +3870,13 @@
         <v>58</v>
       </c>
       <c r="B41" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" t="s">
         <v>149</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>150</v>
-      </c>
-      <c r="D41" t="s">
-        <v>151</v>
       </c>
       <c r="E41" t="s">
         <v>3</v>
@@ -3642,22 +3903,28 @@
         <v>14</v>
       </c>
       <c r="M41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N41">
         <v>0.90000000000000013</v>
       </c>
+      <c r="O41" t="s">
+        <v>285</v>
+      </c>
       <c r="P41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q41" t="s">
         <v>13</v>
       </c>
       <c r="R41" t="s">
+        <v>248</v>
+      </c>
+      <c r="S41" t="s">
         <v>249</v>
       </c>
-      <c r="S41" t="s">
-        <v>250</v>
+      <c r="T41" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="42" spans="1:20">
@@ -3665,10 +3932,10 @@
         <v>59</v>
       </c>
       <c r="B42" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" t="s">
         <v>152</v>
-      </c>
-      <c r="C42" t="s">
-        <v>153</v>
       </c>
       <c r="D42" t="s">
         <v>71</v>
@@ -3677,7 +3944,7 @@
         <v>20</v>
       </c>
       <c r="F42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -3698,13 +3965,28 @@
         <v>14</v>
       </c>
       <c r="M42" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="N42" t="s">
+        <v>285</v>
+      </c>
+      <c r="O42" t="s">
+        <v>285</v>
       </c>
       <c r="P42" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>285</v>
+      </c>
+      <c r="R42" t="s">
         <v>137</v>
       </c>
-      <c r="R42" t="s">
-        <v>138</v>
+      <c r="S42" t="s">
+        <v>285</v>
+      </c>
+      <c r="T42" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="43" spans="1:20">
@@ -3712,19 +3994,19 @@
         <v>62</v>
       </c>
       <c r="B43" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" t="s">
         <v>154</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>155</v>
-      </c>
-      <c r="D43" t="s">
-        <v>156</v>
       </c>
       <c r="E43" t="s">
         <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -3745,16 +4027,28 @@
         <v>10</v>
       </c>
       <c r="M43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N43">
         <v>0.05</v>
       </c>
+      <c r="O43" t="s">
+        <v>285</v>
+      </c>
       <c r="P43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q43" t="s">
-        <v>158</v>
+        <v>157</v>
+      </c>
+      <c r="R43" t="s">
+        <v>285</v>
+      </c>
+      <c r="S43" t="s">
+        <v>285</v>
+      </c>
+      <c r="T43" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="44" spans="1:20">
@@ -3762,10 +4056,10 @@
         <v>67</v>
       </c>
       <c r="B44" t="s">
+        <v>158</v>
+      </c>
+      <c r="C44" t="s">
         <v>159</v>
-      </c>
-      <c r="C44" t="s">
-        <v>160</v>
       </c>
       <c r="D44" t="s">
         <v>71</v>
@@ -3774,7 +4068,7 @@
         <v>20</v>
       </c>
       <c r="F44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -3795,13 +4089,28 @@
         <v>8</v>
       </c>
       <c r="M44" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="N44" t="s">
+        <v>285</v>
+      </c>
+      <c r="O44" t="s">
+        <v>285</v>
       </c>
       <c r="P44" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>285</v>
+      </c>
+      <c r="R44" t="s">
         <v>137</v>
       </c>
-      <c r="R44" t="s">
-        <v>138</v>
+      <c r="S44" t="s">
+        <v>285</v>
+      </c>
+      <c r="T44" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="45" spans="1:20">
@@ -3809,10 +4118,10 @@
         <v>70</v>
       </c>
       <c r="B45" t="s">
+        <v>160</v>
+      </c>
+      <c r="C45" t="s">
         <v>161</v>
-      </c>
-      <c r="C45" t="s">
-        <v>162</v>
       </c>
       <c r="D45" t="s">
         <v>42</v>
@@ -3821,7 +4130,7 @@
         <v>20</v>
       </c>
       <c r="F45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -3842,13 +4151,28 @@
         <v>6</v>
       </c>
       <c r="M45" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="N45" t="s">
+        <v>285</v>
+      </c>
+      <c r="O45" t="s">
+        <v>285</v>
       </c>
       <c r="P45" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>285</v>
+      </c>
+      <c r="R45" t="s">
         <v>137</v>
       </c>
-      <c r="R45" t="s">
-        <v>138</v>
+      <c r="S45" t="s">
+        <v>285</v>
+      </c>
+      <c r="T45" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="46" spans="1:20">
@@ -3856,13 +4180,13 @@
         <v>74</v>
       </c>
       <c r="B46" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" t="s">
         <v>163</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>164</v>
-      </c>
-      <c r="D46" t="s">
-        <v>165</v>
       </c>
       <c r="E46" t="s">
         <v>55</v>
@@ -3889,7 +4213,7 @@
         <v>6</v>
       </c>
       <c r="M46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N46">
         <v>0.35000000000000003</v>
@@ -3898,19 +4222,19 @@
         <v>52</v>
       </c>
       <c r="P46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R46" t="s">
+        <v>250</v>
+      </c>
+      <c r="S46" t="s">
         <v>251</v>
       </c>
-      <c r="S46" t="s">
-        <v>252</v>
-      </c>
       <c r="T46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:20">
@@ -3918,13 +4242,13 @@
         <v>78</v>
       </c>
       <c r="B47" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47" t="s">
         <v>167</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>168</v>
-      </c>
-      <c r="D47" t="s">
-        <v>169</v>
       </c>
       <c r="E47" t="s">
         <v>20</v>
@@ -3932,23 +4256,47 @@
       <c r="F47" t="s">
         <v>37</v>
       </c>
+      <c r="G47" t="s">
+        <v>285</v>
+      </c>
+      <c r="H47" t="s">
+        <v>285</v>
+      </c>
+      <c r="I47" t="s">
+        <v>285</v>
+      </c>
+      <c r="J47" t="s">
+        <v>285</v>
+      </c>
+      <c r="K47" t="s">
+        <v>285</v>
+      </c>
+      <c r="L47" t="s">
+        <v>285</v>
+      </c>
       <c r="M47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N47">
         <v>0.05</v>
       </c>
+      <c r="O47" t="s">
+        <v>285</v>
+      </c>
       <c r="P47" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q47" t="s">
         <v>13</v>
       </c>
       <c r="R47" t="s">
+        <v>252</v>
+      </c>
+      <c r="S47" t="s">
         <v>253</v>
       </c>
-      <c r="S47" t="s">
-        <v>254</v>
+      <c r="T47" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="48" spans="1:20">
@@ -3956,13 +4304,13 @@
         <v>79</v>
       </c>
       <c r="B48" t="s">
+        <v>169</v>
+      </c>
+      <c r="C48" t="s">
         <v>170</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>171</v>
-      </c>
-      <c r="D48" t="s">
-        <v>172</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
@@ -3989,7 +4337,7 @@
         <v>6</v>
       </c>
       <c r="M48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N48">
         <v>0.15000000000000002</v>
@@ -3998,19 +4346,19 @@
         <v>52</v>
       </c>
       <c r="P48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q48" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R48" t="s">
+        <v>254</v>
+      </c>
+      <c r="S48" t="s">
         <v>255</v>
       </c>
-      <c r="S48" t="s">
-        <v>256</v>
-      </c>
       <c r="T48" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:20">
@@ -4018,13 +4366,13 @@
         <v>83</v>
       </c>
       <c r="B49" t="s">
+        <v>173</v>
+      </c>
+      <c r="C49" t="s">
         <v>174</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>175</v>
-      </c>
-      <c r="D49" t="s">
-        <v>176</v>
       </c>
       <c r="E49" t="s">
         <v>3</v>
@@ -4032,26 +4380,47 @@
       <c r="F49" t="s">
         <v>37</v>
       </c>
+      <c r="G49" t="s">
+        <v>285</v>
+      </c>
+      <c r="H49" t="s">
+        <v>285</v>
+      </c>
+      <c r="I49" t="s">
+        <v>285</v>
+      </c>
+      <c r="J49" t="s">
+        <v>285</v>
+      </c>
+      <c r="K49" t="s">
+        <v>285</v>
+      </c>
+      <c r="L49" t="s">
+        <v>285</v>
+      </c>
       <c r="M49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N49">
         <v>0.35</v>
       </c>
+      <c r="O49" t="s">
+        <v>285</v>
+      </c>
       <c r="P49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R49" t="s">
+        <v>256</v>
+      </c>
+      <c r="S49" t="s">
         <v>257</v>
       </c>
-      <c r="S49" t="s">
-        <v>258</v>
-      </c>
       <c r="T49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:20">
@@ -4059,10 +4428,13 @@
         <v>84</v>
       </c>
       <c r="B50" t="s">
+        <v>177</v>
+      </c>
+      <c r="C50" t="s">
+        <v>285</v>
+      </c>
+      <c r="D50" t="s">
         <v>178</v>
-      </c>
-      <c r="D50" t="s">
-        <v>179</v>
       </c>
       <c r="E50" t="s">
         <v>3</v>
@@ -4070,17 +4442,47 @@
       <c r="F50" t="s">
         <v>4</v>
       </c>
+      <c r="G50" t="s">
+        <v>285</v>
+      </c>
+      <c r="H50" t="s">
+        <v>285</v>
+      </c>
+      <c r="I50" t="s">
+        <v>285</v>
+      </c>
+      <c r="J50" t="s">
+        <v>285</v>
+      </c>
+      <c r="K50" t="s">
+        <v>285</v>
+      </c>
+      <c r="L50" t="s">
+        <v>285</v>
+      </c>
       <c r="M50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N50">
         <v>0.9</v>
       </c>
+      <c r="O50" t="s">
+        <v>285</v>
+      </c>
       <c r="P50" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q50" t="s">
         <v>180</v>
       </c>
-      <c r="Q50" t="s">
-        <v>181</v>
+      <c r="R50" t="s">
+        <v>285</v>
+      </c>
+      <c r="S50" t="s">
+        <v>285</v>
+      </c>
+      <c r="T50" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="51" spans="1:20">
@@ -4088,13 +4490,13 @@
         <v>85</v>
       </c>
       <c r="B51" t="s">
+        <v>181</v>
+      </c>
+      <c r="C51" t="s">
         <v>182</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>183</v>
-      </c>
-      <c r="D51" t="s">
-        <v>184</v>
       </c>
       <c r="E51" t="s">
         <v>20</v>
@@ -4102,26 +4504,47 @@
       <c r="F51" t="s">
         <v>37</v>
       </c>
+      <c r="G51" t="s">
+        <v>285</v>
+      </c>
+      <c r="H51" t="s">
+        <v>285</v>
+      </c>
+      <c r="I51" t="s">
+        <v>285</v>
+      </c>
+      <c r="J51" t="s">
+        <v>285</v>
+      </c>
+      <c r="K51" t="s">
+        <v>285</v>
+      </c>
+      <c r="L51" t="s">
+        <v>285</v>
+      </c>
       <c r="M51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N51">
         <v>0.25</v>
       </c>
+      <c r="O51" t="s">
+        <v>285</v>
+      </c>
       <c r="P51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q51" t="s">
+        <v>184</v>
+      </c>
+      <c r="R51" t="s">
+        <v>258</v>
+      </c>
+      <c r="S51" t="s">
+        <v>259</v>
+      </c>
+      <c r="T51" t="s">
         <v>185</v>
-      </c>
-      <c r="R51" t="s">
-        <v>259</v>
-      </c>
-      <c r="S51" t="s">
-        <v>260</v>
-      </c>
-      <c r="T51" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="52" spans="1:20">
@@ -4129,10 +4552,13 @@
         <v>86</v>
       </c>
       <c r="B52" t="s">
+        <v>186</v>
+      </c>
+      <c r="C52" t="s">
+        <v>285</v>
+      </c>
+      <c r="D52" t="s">
         <v>187</v>
-      </c>
-      <c r="D52" t="s">
-        <v>188</v>
       </c>
       <c r="E52" t="s">
         <v>20</v>
@@ -4140,26 +4566,47 @@
       <c r="F52" t="s">
         <v>37</v>
       </c>
+      <c r="G52" t="s">
+        <v>285</v>
+      </c>
+      <c r="H52" t="s">
+        <v>285</v>
+      </c>
+      <c r="I52" t="s">
+        <v>285</v>
+      </c>
+      <c r="J52" t="s">
+        <v>285</v>
+      </c>
+      <c r="K52" t="s">
+        <v>285</v>
+      </c>
+      <c r="L52" t="s">
+        <v>285</v>
+      </c>
       <c r="M52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N52">
         <v>0.45</v>
       </c>
+      <c r="O52" t="s">
+        <v>285</v>
+      </c>
       <c r="P52" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q52" t="s">
         <v>13</v>
       </c>
       <c r="R52" t="s">
+        <v>260</v>
+      </c>
+      <c r="S52" t="s">
         <v>261</v>
       </c>
-      <c r="S52" t="s">
-        <v>262</v>
-      </c>
       <c r="T52" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="53" spans="1:20">
@@ -4167,10 +4614,10 @@
         <v>87</v>
       </c>
       <c r="B53" t="s">
+        <v>189</v>
+      </c>
+      <c r="C53" t="s">
         <v>190</v>
-      </c>
-      <c r="C53" t="s">
-        <v>191</v>
       </c>
       <c r="D53" t="s">
         <v>42</v>
@@ -4200,7 +4647,7 @@
         <v>19</v>
       </c>
       <c r="M53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N53">
         <v>0.1</v>
@@ -4209,19 +4656,19 @@
         <v>6</v>
       </c>
       <c r="P53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q53" t="s">
+        <v>191</v>
+      </c>
+      <c r="R53" t="s">
+        <v>262</v>
+      </c>
+      <c r="S53" t="s">
+        <v>263</v>
+      </c>
+      <c r="T53" t="s">
         <v>192</v>
-      </c>
-      <c r="R53" t="s">
-        <v>263</v>
-      </c>
-      <c r="S53" t="s">
-        <v>264</v>
-      </c>
-      <c r="T53" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="54" spans="1:20">
@@ -4229,28 +4676,61 @@
         <v>88</v>
       </c>
       <c r="B54" t="s">
+        <v>193</v>
+      </c>
+      <c r="C54" t="s">
         <v>194</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
+        <v>183</v>
+      </c>
+      <c r="E54" t="s">
         <v>195</v>
       </c>
-      <c r="D54" t="s">
-        <v>184</v>
-      </c>
-      <c r="E54" t="s">
-        <v>196</v>
-      </c>
       <c r="F54" t="s">
-        <v>196</v>
+        <v>195</v>
+      </c>
+      <c r="G54" t="s">
+        <v>285</v>
+      </c>
+      <c r="H54" t="s">
+        <v>285</v>
+      </c>
+      <c r="I54" t="s">
+        <v>285</v>
+      </c>
+      <c r="J54" t="s">
+        <v>285</v>
+      </c>
+      <c r="K54" t="s">
+        <v>285</v>
+      </c>
+      <c r="L54" t="s">
+        <v>285</v>
       </c>
       <c r="M54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N54">
         <v>0</v>
       </c>
+      <c r="O54" t="s">
+        <v>285</v>
+      </c>
+      <c r="P54" t="s">
+        <v>285</v>
+      </c>
       <c r="Q54" t="s">
-        <v>185</v>
+        <v>184</v>
+      </c>
+      <c r="R54" t="s">
+        <v>285</v>
+      </c>
+      <c r="S54" t="s">
+        <v>285</v>
+      </c>
+      <c r="T54" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="55" spans="1:20">
@@ -4258,10 +4738,10 @@
         <v>89</v>
       </c>
       <c r="B55" t="s">
+        <v>196</v>
+      </c>
+      <c r="C55" t="s">
         <v>197</v>
-      </c>
-      <c r="C55" t="s">
-        <v>198</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
@@ -4291,7 +4771,7 @@
         <v>21</v>
       </c>
       <c r="M55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N55">
         <v>0.15</v>
@@ -4300,19 +4780,19 @@
         <v>52</v>
       </c>
       <c r="P55" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q55" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R55" t="s">
+        <v>264</v>
+      </c>
+      <c r="S55" t="s">
         <v>265</v>
       </c>
-      <c r="S55" t="s">
-        <v>266</v>
-      </c>
       <c r="T55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>